<commit_message>
Changed how the PGAVSS was handled
</commit_message>
<xml_diff>
--- a/RA6M3 Pinout.xlsx
+++ b/RA6M3 Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Dropbox\CraigCo\Internal\Projects\MCU Combinatorics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717B3E83-DDA1-4C79-8658-EAA027E5E73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A719C2-5282-4F24-A2B7-0AEB579EF1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44880" yWindow="-4290" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{72AD40F7-C012-4E82-829B-31755AFA1EBE}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9187" uniqueCount="1229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9189" uniqueCount="1229">
   <si>
     <t>SWCLK</t>
   </si>
@@ -3859,7 +3859,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3907,9 +3907,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4231,10 +4228,10 @@
   <dimension ref="A1:AB186"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B134" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="Y94" sqref="Y94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19946,10 +19943,10 @@
   <dimension ref="A1:I791"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19959,11 +19956,11 @@
     <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>915</v>
       </c>
@@ -20758,11 +20755,11 @@
       <c r="F31" s="5" t="s">
         <v>1124</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="16" t="s">
+        <v>1227</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>1125</v>
-      </c>
-      <c r="H31" s="16">
-        <v>0</v>
       </c>
       <c r="I31" s="16"/>
     </row>
@@ -20785,11 +20782,11 @@
       <c r="F32" s="5" t="s">
         <v>1124</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="16" t="s">
+        <v>1228</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>1125</v>
-      </c>
-      <c r="H32" s="16">
-        <v>1</v>
       </c>
       <c r="I32" s="16"/>
     </row>
@@ -32073,19 +32070,19 @@
       <c r="I433" s="16"/>
     </row>
     <row r="434" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A434" s="18" t="s">
+      <c r="A434" s="5" t="s">
         <v>1048</v>
       </c>
-      <c r="B434" s="18">
+      <c r="B434" s="5">
         <v>1</v>
       </c>
-      <c r="C434" s="18" t="s">
+      <c r="C434" s="5" t="s">
         <v>1048</v>
       </c>
-      <c r="D434" s="18">
+      <c r="D434" s="5">
         <v>1</v>
       </c>
-      <c r="E434" s="18">
+      <c r="E434" s="5">
         <v>1</v>
       </c>
       <c r="F434" s="16" t="s">
@@ -32102,19 +32099,19 @@
       </c>
     </row>
     <row r="435" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A435" s="18" t="s">
+      <c r="A435" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="B435" s="18">
+      <c r="B435" s="5">
         <v>43</v>
       </c>
-      <c r="C435" s="18" t="s">
+      <c r="C435" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="D435" s="18">
+      <c r="D435" s="5">
         <v>35</v>
       </c>
-      <c r="E435" s="18">
+      <c r="E435" s="5">
         <v>24</v>
       </c>
       <c r="F435" s="16" t="s">
@@ -32131,19 +32128,19 @@
       </c>
     </row>
     <row r="436" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A436" s="18" t="s">
+      <c r="A436" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="B436" s="18">
+      <c r="B436" s="5">
         <v>52</v>
       </c>
-      <c r="C436" s="18" t="s">
+      <c r="C436" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="D436" s="18">
+      <c r="D436" s="5">
         <v>44</v>
       </c>
-      <c r="E436" s="18" t="s">
+      <c r="E436" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F436" s="16" t="s">
@@ -32160,19 +32157,19 @@
       </c>
     </row>
     <row r="437" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A437" s="18" t="s">
+      <c r="A437" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="B437" s="18">
+      <c r="B437" s="5">
         <v>51</v>
       </c>
-      <c r="C437" s="18" t="s">
+      <c r="C437" s="5" t="s">
         <v>989</v>
       </c>
-      <c r="D437" s="18">
+      <c r="D437" s="5">
         <v>43</v>
       </c>
-      <c r="E437" s="18">
+      <c r="E437" s="5">
         <v>32</v>
       </c>
       <c r="F437" s="16" t="s">
@@ -32189,19 +32186,19 @@
       </c>
     </row>
     <row r="438" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A438" s="18" t="s">
+      <c r="A438" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="B438" s="18">
+      <c r="B438" s="5">
         <v>132</v>
       </c>
-      <c r="C438" s="18" t="s">
+      <c r="C438" s="5" t="s">
         <v>960</v>
       </c>
-      <c r="D438" s="18">
+      <c r="D438" s="5">
         <v>108</v>
       </c>
-      <c r="E438" s="18">
+      <c r="E438" s="5">
         <v>75</v>
       </c>
       <c r="F438" s="16" t="s">
@@ -32218,19 +32215,19 @@
       </c>
     </row>
     <row r="439" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A439" s="18" t="s">
+      <c r="A439" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="B439" s="18">
+      <c r="B439" s="5">
         <v>175</v>
       </c>
-      <c r="C439" s="18" t="s">
+      <c r="C439" s="5" t="s">
         <v>1026</v>
       </c>
-      <c r="D439" s="18">
+      <c r="D439" s="5">
         <v>143</v>
       </c>
-      <c r="E439" s="18" t="s">
+      <c r="E439" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F439" s="16" t="s">
@@ -32245,19 +32242,19 @@
       <c r="I439" s="16"/>
     </row>
     <row r="440" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A440" s="18" t="s">
+      <c r="A440" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="B440" s="18">
+      <c r="B440" s="5">
         <v>2</v>
       </c>
-      <c r="C440" s="18" t="s">
+      <c r="C440" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="D440" s="18">
+      <c r="D440" s="5">
         <v>2</v>
       </c>
-      <c r="E440" s="18">
+      <c r="E440" s="5">
         <v>2</v>
       </c>
       <c r="F440" s="16" t="s">
@@ -32274,19 +32271,19 @@
       </c>
     </row>
     <row r="441" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A441" s="18" t="s">
+      <c r="A441" s="5" t="s">
         <v>974</v>
       </c>
-      <c r="B441" s="18">
+      <c r="B441" s="5">
         <v>44</v>
       </c>
-      <c r="C441" s="18" t="s">
+      <c r="C441" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="D441" s="18">
+      <c r="D441" s="5">
         <v>36</v>
       </c>
-      <c r="E441" s="18">
+      <c r="E441" s="5">
         <v>25</v>
       </c>
       <c r="F441" s="16" t="s">
@@ -32303,19 +32300,19 @@
       </c>
     </row>
     <row r="442" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A442" s="18" t="s">
+      <c r="A442" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="B442" s="18">
+      <c r="B442" s="5">
         <v>50</v>
       </c>
-      <c r="C442" s="18" t="s">
+      <c r="C442" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="D442" s="18">
+      <c r="D442" s="5">
         <v>42</v>
       </c>
-      <c r="E442" s="18">
+      <c r="E442" s="5">
         <v>31</v>
       </c>
       <c r="F442" s="16" t="s">
@@ -32332,19 +32329,19 @@
       </c>
     </row>
     <row r="443" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A443" s="18" t="s">
+      <c r="A443" s="5" t="s">
         <v>962</v>
       </c>
-      <c r="B443" s="18">
+      <c r="B443" s="5">
         <v>131</v>
       </c>
-      <c r="C443" s="18" t="s">
+      <c r="C443" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="D443" s="18">
+      <c r="D443" s="5">
         <v>107</v>
       </c>
-      <c r="E443" s="18">
+      <c r="E443" s="5">
         <v>74</v>
       </c>
       <c r="F443" s="16" t="s">
@@ -32361,19 +32358,19 @@
       </c>
     </row>
     <row r="444" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A444" s="18" t="s">
+      <c r="A444" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="B444" s="18">
+      <c r="B444" s="5">
         <v>176</v>
       </c>
-      <c r="C444" s="18" t="s">
+      <c r="C444" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="D444" s="18">
+      <c r="D444" s="5">
         <v>144</v>
       </c>
-      <c r="E444" s="18" t="s">
+      <c r="E444" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F444" s="16" t="s">
@@ -37947,19 +37944,19 @@
       </c>
     </row>
     <row r="644" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A644" s="19" t="s">
+      <c r="A644" s="18" t="s">
         <v>966</v>
       </c>
-      <c r="B644" s="19">
+      <c r="B644" s="18">
         <v>53</v>
       </c>
-      <c r="C644" s="19" t="s">
+      <c r="C644" s="18" t="s">
         <v>967</v>
       </c>
-      <c r="D644" s="19">
+      <c r="D644" s="18">
         <v>45</v>
       </c>
-      <c r="E644" s="19" t="s">
+      <c r="E644" s="18" t="s">
         <v>4</v>
       </c>
       <c r="F644" s="5" t="s">

</xml_diff>